<commit_message>
filled in table 1 w/ values from models
</commit_message>
<xml_diff>
--- a/table 1.xlsx
+++ b/table 1.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Appendix E" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Model</t>
   </si>
@@ -28,12 +29,6 @@
     <t>Segmented logistic regression</t>
   </si>
   <si>
-    <t>Segment 1: &lt;0.XXXX mg P/L</t>
-  </si>
-  <si>
-    <t>Segment 2: &gt;0.XXXX mg P/L</t>
-  </si>
-  <si>
     <t>Partitioned logistic regression</t>
   </si>
   <si>
@@ -56,13 +51,51 @@
   </si>
   <si>
     <t>Relationship between total phosphorus &amp; floating plant cover</t>
+  </si>
+  <si>
+    <t>Residual deviance</t>
+  </si>
+  <si>
+    <t>Segment 1: &lt;0.0.3698 mg P/L</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Segment 2: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>≥</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>0.03698 mg P/L</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT ADDITIVE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNSURE IF THESE SHOULD BE ADDED </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -81,6 +114,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -128,6 +167,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -431,88 +473,157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="A1:C8"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="6"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6">
+        <v>43.713000000000001</v>
+      </c>
+      <c r="D2" s="6">
+        <v>69.397999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6">
+        <v>42.384</v>
+      </c>
+      <c r="D3" s="6">
+        <v>69.090999999999994</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6">
+        <v>8.7729999999999997</v>
+      </c>
+      <c r="D4" s="6">
+        <v>20.846</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="6">
+        <v>31.318000000000001</v>
+      </c>
+      <c r="D5" s="6">
+        <v>46.261000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C6" s="7">
+        <f>SUM(C7:C8)</f>
+        <v>11.783200000000001</v>
+      </c>
+      <c r="D6" s="7">
+        <f>SUM(D7:D8)</f>
+        <v>27.089599999999997</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3.22</v>
+      </c>
+      <c r="D7" s="6">
+        <v>6.4105999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="B8" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8.5632000000000001</v>
+      </c>
+      <c r="D8" s="6">
+        <v>20.678999999999998</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>